<commit_message>
7-25 change combo-op input-op operation
</commit_message>
<xml_diff>
--- a/data/easy.xlsx
+++ b/data/easy.xlsx
@@ -66,6 +66,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -3221,10 +3289,8 @@
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="B22" t="n">
+        <v>10</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -3291,20 +3357,16 @@
           <t>热控计算机</t>
         </is>
       </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>1315.0</t>
-        </is>
+      <c r="P22" t="n">
+        <v>1315</v>
       </c>
       <c r="Q22" t="inlineStr">
         <is>
           <t>热力机械工作票</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="R22" t="n">
+        <v>2</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>

</xml_diff>